<commit_message>
update w10 plus videos
</commit_message>
<xml_diff>
--- a/articles/course_docs/data_2024_schedule.xlsx
+++ b/articles/course_docs/data_2024_schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.kumar/Documents/data-analysis/articles/course_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/Desktop/data-analysis/articles/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC79264-1B26-6248-8281-9ADBE7B8DA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88286F5A-5E7E-D545-BCFC-1FB356E02597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>&lt;b&gt;&lt;span style="color:#8304BA"&gt; Problem Set 4 due / Opt-out Deadline 2&lt;/span&gt;&lt;/b&gt;</t>
   </si>
   <si>
-    <t>T: March 12, 2024</t>
-  </si>
-  <si>
     <t>T: April 2, 2024</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>T: April 23, 2024</t>
+  </si>
+  <si>
+    <t>T: March 26, 2024</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XEY40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9049,15 +9049,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34">
+    <row r="19" spans="1:3" ht="18">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18">
@@ -9065,7 +9065,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>41</v>
@@ -9073,10 +9073,10 @@
     </row>
     <row r="21" spans="1:3" ht="18">
       <c r="A21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>41</v>
@@ -9087,21 +9087,21 @@
         <v>9</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18">
+    <row r="23" spans="1:3" ht="34">
       <c r="A23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>41</v>
+        <v>77</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18">
@@ -9131,7 +9131,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>66</v>
@@ -9164,7 +9164,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>67</v>
@@ -9219,7 +9219,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>71</v>

</xml_diff>